<commit_message>
builds to latest/ with release to version folder possible
</commit_message>
<xml_diff>
--- a/nomenclature_parser/in/Nomenclatures EMSI EVENT.xlsx
+++ b/nomenclature_parser/in/Nomenclatures EMSI EVENT.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27108"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="11010"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://esantegouv.sharepoint.com/sites/GED-Calypso/espace-projets/Espace Programme SISAMU/01 - Equipe projet/07 - Innovation et prospectif/12 - Hub Santé/17 - MDD/Nomenclatures/01 - Base interne/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://esantegouv.sharepoint.com/sites/GED-Calypso/espace-projets/Espace Programme SISAMU/01 - Equipe projet/07 - Innovation et prospectif/12 - Hub Santé/17 - MDD/Nomenclatures/01 - Base interne/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="882" documentId="13_ncr:1_{420DE2DB-F177-420D-9F91-385C2DF0C062}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{5D5A8077-B32C-4885-AEC1-B370F5FC3E5B}"/>
+  <xr:revisionPtr revIDLastSave="884" documentId="13_ncr:1_{420DE2DB-F177-420D-9F91-385C2DF0C062}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{C536996A-4D50-FC45-90DD-15C8F77C2A33}"/>
   <bookViews>
-    <workbookView minimized="1" xWindow="31965" yWindow="2640" windowWidth="21600" windowHeight="11295" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2680" yWindow="-20640" windowWidth="34560" windowHeight="20160" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="EVENT.ETYPE.CATEGORY" sheetId="9" r:id="rId1"/>
@@ -3935,6 +3935,41 @@
     <cellStyle name="Normal 2" xfId="2" xr:uid="{289B6461-38A1-47EB-AD2F-3A7ED8C77D6E}"/>
   </cellStyles>
   <dxfs count="79">
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="8"/>
+        <color auto="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
     <dxf>
       <font>
         <b val="0"/>
@@ -5153,41 +5188,6 @@
         <family val="2"/>
         <scheme val="minor"/>
       </font>
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="8"/>
-        <color auto="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
       <border diagonalUp="0" diagonalDown="0">
         <left style="thin">
           <color indexed="64"/>
@@ -5983,40 +5983,40 @@
 </file>
 
 <file path=xl/tables/table10.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="12" xr:uid="{26DF3307-34F4-42AE-84A4-0D4CBF066D54}" name="Table134579111213" displayName="Table134579111213" ref="A9:E57" totalsRowShown="0" headerRowDxfId="18" dataDxfId="17">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="12" xr:uid="{26DF3307-34F4-42AE-84A4-0D4CBF066D54}" name="Table134579111213" displayName="Table134579111213" ref="A9:E57" totalsRowShown="0" headerRowDxfId="19" dataDxfId="18">
   <autoFilter ref="A9:E57" xr:uid="{B3C2A837-EDE7-4BB4-94EB-1FCD3E6C6353}"/>
   <tableColumns count="5">
-    <tableColumn id="1" xr3:uid="{26EE7CCE-0A08-4908-A677-59C683486D38}" name="Code" dataDxfId="16"/>
-    <tableColumn id="2" xr3:uid="{CDC16B11-DD37-446F-8F21-E3D9026DD97C}" name="Libellé niveau 1" dataDxfId="15"/>
-    <tableColumn id="5" xr3:uid="{A51DB763-9299-451D-A810-BCEA65D9E01D}" name="Libellé niveau 2" dataDxfId="14"/>
-    <tableColumn id="3" xr3:uid="{A4FF1C94-E2C0-4BEC-A828-8B7732E4CD60}" name="Description" dataDxfId="13"/>
-    <tableColumn id="4" xr3:uid="{C1E7BA75-D90A-44E9-823B-A6443FBAB216}" name="Commentaire" dataDxfId="12"/>
+    <tableColumn id="1" xr3:uid="{26EE7CCE-0A08-4908-A677-59C683486D38}" name="Code" dataDxfId="17"/>
+    <tableColumn id="2" xr3:uid="{CDC16B11-DD37-446F-8F21-E3D9026DD97C}" name="Libellé niveau 1" dataDxfId="16"/>
+    <tableColumn id="5" xr3:uid="{A51DB763-9299-451D-A810-BCEA65D9E01D}" name="Libellé niveau 2" dataDxfId="15"/>
+    <tableColumn id="3" xr3:uid="{A4FF1C94-E2C0-4BEC-A828-8B7732E4CD60}" name="Description" dataDxfId="14"/>
+    <tableColumn id="4" xr3:uid="{C1E7BA75-D90A-44E9-823B-A6443FBAB216}" name="Commentaire" dataDxfId="13"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table11.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="10" xr:uid="{CDF36831-79C4-46E2-A8A4-A2D002055482}" name="Table13457911" displayName="Table13457911" ref="A9:D15" totalsRowShown="0" headerRowDxfId="11" dataDxfId="10">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="10" xr:uid="{CDF36831-79C4-46E2-A8A4-A2D002055482}" name="Table13457911" displayName="Table13457911" ref="A9:D15" totalsRowShown="0" headerRowDxfId="12" dataDxfId="11">
   <autoFilter ref="A9:D15" xr:uid="{CDF36831-79C4-46E2-A8A4-A2D002055482}"/>
   <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{827CD47C-54B9-492C-BEC1-38B3CBDEA92E}" name="Code" dataDxfId="9"/>
-    <tableColumn id="2" xr3:uid="{B7ADDE36-930D-429D-B06C-F6B843153C60}" name="Libellé niveau 1" dataDxfId="8"/>
-    <tableColumn id="3" xr3:uid="{DB478352-58AC-4CF9-AEB7-17CD612D9C64}" name="Description" dataDxfId="7"/>
-    <tableColumn id="4" xr3:uid="{63664487-54C4-4FB8-9A75-EE1F75C736C2}" name="Commentaire" dataDxfId="6"/>
+    <tableColumn id="1" xr3:uid="{827CD47C-54B9-492C-BEC1-38B3CBDEA92E}" name="Code" dataDxfId="10"/>
+    <tableColumn id="2" xr3:uid="{B7ADDE36-930D-429D-B06C-F6B843153C60}" name="Libellé niveau 1" dataDxfId="9"/>
+    <tableColumn id="3" xr3:uid="{DB478352-58AC-4CF9-AEB7-17CD612D9C64}" name="Description" dataDxfId="8"/>
+    <tableColumn id="4" xr3:uid="{63664487-54C4-4FB8-9A75-EE1F75C736C2}" name="Commentaire" dataDxfId="7"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table12.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="11" xr:uid="{B3C2A837-EDE7-4BB4-94EB-1FCD3E6C6353}" name="Table1345791112" displayName="Table1345791112" ref="A9:D12" totalsRowShown="0" headerRowDxfId="5" dataDxfId="4">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="11" xr:uid="{B3C2A837-EDE7-4BB4-94EB-1FCD3E6C6353}" name="Table1345791112" displayName="Table1345791112" ref="A9:D12" totalsRowShown="0" headerRowDxfId="6" dataDxfId="5">
   <autoFilter ref="A9:D12" xr:uid="{B3C2A837-EDE7-4BB4-94EB-1FCD3E6C6353}"/>
   <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{FF144121-7487-4B50-8A65-49A8AC28EBBC}" name="Code" dataDxfId="3"/>
-    <tableColumn id="2" xr3:uid="{419998F0-6C22-4337-887A-52DAD4433A40}" name="Libellé niveau 1" dataDxfId="2"/>
-    <tableColumn id="3" xr3:uid="{30E5AAA1-E57D-4F0A-AE50-7AE2BAEBE289}" name="Description" dataDxfId="1"/>
-    <tableColumn id="4" xr3:uid="{4BFF9456-387C-4FEC-94E6-13FEF83002CF}" name="Commentaire" dataDxfId="0"/>
+    <tableColumn id="1" xr3:uid="{FF144121-7487-4B50-8A65-49A8AC28EBBC}" name="Code" dataDxfId="4"/>
+    <tableColumn id="2" xr3:uid="{419998F0-6C22-4337-887A-52DAD4433A40}" name="Libellé niveau 1" dataDxfId="3"/>
+    <tableColumn id="3" xr3:uid="{30E5AAA1-E57D-4F0A-AE50-7AE2BAEBE289}" name="Description" dataDxfId="2"/>
+    <tableColumn id="4" xr3:uid="{4BFF9456-387C-4FEC-94E6-13FEF83002CF}" name="Commentaire" dataDxfId="1"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -6071,61 +6071,61 @@
   <tableColumns count="4">
     <tableColumn id="1" xr3:uid="{5F5C37BB-9414-45F4-882F-C30DBF6693A5}" name="Code" dataDxfId="47"/>
     <tableColumn id="2" xr3:uid="{8CC3DA00-B777-4A14-9918-8E544FEE762C}" name="Libellé niveau 1" dataDxfId="46"/>
-    <tableColumn id="3" xr3:uid="{22407615-9D4D-48D6-B548-25DBB05445D9}" name="Description" dataDxfId="45"/>
-    <tableColumn id="4" xr3:uid="{457E12C2-4B88-45D4-BB7E-F312B1CD816C}" name="Commentaire" dataDxfId="44"/>
+    <tableColumn id="3" xr3:uid="{22407615-9D4D-48D6-B548-25DBB05445D9}" name="Description" dataDxfId="0"/>
+    <tableColumn id="4" xr3:uid="{457E12C2-4B88-45D4-BB7E-F312B1CD816C}" name="Commentaire" dataDxfId="45"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="7" xr:uid="{1BA9C99E-0FEA-4661-A32A-C70E83B4A5DF}" name="Table134578" displayName="Table134578" ref="A9:D14" totalsRowShown="0" headerRowDxfId="43" dataDxfId="42">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="7" xr:uid="{1BA9C99E-0FEA-4661-A32A-C70E83B4A5DF}" name="Table134578" displayName="Table134578" ref="A9:D14" totalsRowShown="0" headerRowDxfId="44" dataDxfId="43">
   <autoFilter ref="A9:D14" xr:uid="{1BA9C99E-0FEA-4661-A32A-C70E83B4A5DF}"/>
   <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{5D7488F6-CDA9-48C2-A99F-2DE474359121}" name="Code" dataDxfId="41"/>
-    <tableColumn id="2" xr3:uid="{AE5DDD33-6682-42EF-85AC-99A3CAC427CE}" name="Libellé niveau 1" dataDxfId="40"/>
-    <tableColumn id="3" xr3:uid="{BE555B52-6698-4900-A795-2697B7BF98AE}" name="Description" dataDxfId="39"/>
-    <tableColumn id="4" xr3:uid="{FBA181AC-8F3F-4A9C-9A04-E19FDB35DE0E}" name="Commentaire" dataDxfId="38"/>
+    <tableColumn id="1" xr3:uid="{5D7488F6-CDA9-48C2-A99F-2DE474359121}" name="Code" dataDxfId="42"/>
+    <tableColumn id="2" xr3:uid="{AE5DDD33-6682-42EF-85AC-99A3CAC427CE}" name="Libellé niveau 1" dataDxfId="41"/>
+    <tableColumn id="3" xr3:uid="{BE555B52-6698-4900-A795-2697B7BF98AE}" name="Description" dataDxfId="40"/>
+    <tableColumn id="4" xr3:uid="{FBA181AC-8F3F-4A9C-9A04-E19FDB35DE0E}" name="Commentaire" dataDxfId="39"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table7.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{9BBAEC71-98FF-4AB8-B5E1-1CE8C8584409}" name="Table1345" displayName="Table1345" ref="A9:D13" totalsRowShown="0" headerRowDxfId="37" dataDxfId="36">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{9BBAEC71-98FF-4AB8-B5E1-1CE8C8584409}" name="Table1345" displayName="Table1345" ref="A9:D13" totalsRowShown="0" headerRowDxfId="38" dataDxfId="37">
   <autoFilter ref="A9:D13" xr:uid="{9BBAEC71-98FF-4AB8-B5E1-1CE8C8584409}"/>
   <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{CC3785D5-DB9A-4D60-862F-F8E090985E56}" name="Code" dataDxfId="35"/>
-    <tableColumn id="2" xr3:uid="{0E29D007-DD2B-4361-B0B6-3124B15DD8DA}" name="Libellé niveau 1" dataDxfId="34"/>
-    <tableColumn id="3" xr3:uid="{2F058103-5AD9-4F2B-A662-54DD0A6EEAE9}" name="Description" dataDxfId="33"/>
-    <tableColumn id="4" xr3:uid="{E9F88BD4-157D-4840-B9EE-0122B96E7D08}" name="Commentaire" dataDxfId="32"/>
+    <tableColumn id="1" xr3:uid="{CC3785D5-DB9A-4D60-862F-F8E090985E56}" name="Code" dataDxfId="36"/>
+    <tableColumn id="2" xr3:uid="{0E29D007-DD2B-4361-B0B6-3124B15DD8DA}" name="Libellé niveau 1" dataDxfId="35"/>
+    <tableColumn id="3" xr3:uid="{2F058103-5AD9-4F2B-A662-54DD0A6EEAE9}" name="Description" dataDxfId="34"/>
+    <tableColumn id="4" xr3:uid="{E9F88BD4-157D-4840-B9EE-0122B96E7D08}" name="Commentaire" dataDxfId="33"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table8.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="8" xr:uid="{448164F5-1D63-43E2-8F84-C919457EC610}" name="Table134579" displayName="Table134579" ref="A9:D12" totalsRowShown="0" headerRowDxfId="31" dataDxfId="30">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="8" xr:uid="{448164F5-1D63-43E2-8F84-C919457EC610}" name="Table134579" displayName="Table134579" ref="A9:D12" totalsRowShown="0" headerRowDxfId="32" dataDxfId="31">
   <autoFilter ref="A9:D12" xr:uid="{448164F5-1D63-43E2-8F84-C919457EC610}"/>
   <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{033E47FB-ADF9-40CF-A20D-BF29E04ADB55}" name="Code" dataDxfId="29"/>
-    <tableColumn id="2" xr3:uid="{E55A0DD3-BD4F-4DD2-A60D-BB8F4A8862C6}" name="Libellé niveau 1" dataDxfId="28"/>
-    <tableColumn id="3" xr3:uid="{9682D9C0-6A4A-45B9-BAFE-9ADE23B9A964}" name="Description" dataDxfId="27"/>
-    <tableColumn id="4" xr3:uid="{6EDEDC97-62DF-432C-8466-D8B59200DD75}" name="Commentaire" dataDxfId="26"/>
+    <tableColumn id="1" xr3:uid="{033E47FB-ADF9-40CF-A20D-BF29E04ADB55}" name="Code" dataDxfId="30"/>
+    <tableColumn id="2" xr3:uid="{E55A0DD3-BD4F-4DD2-A60D-BB8F4A8862C6}" name="Libellé niveau 1" dataDxfId="29"/>
+    <tableColumn id="3" xr3:uid="{9682D9C0-6A4A-45B9-BAFE-9ADE23B9A964}" name="Description" dataDxfId="28"/>
+    <tableColumn id="4" xr3:uid="{6EDEDC97-62DF-432C-8466-D8B59200DD75}" name="Commentaire" dataDxfId="27"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table9.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="9" xr:uid="{25A0FEFF-9550-49E1-8274-9CC0D23D601A}" name="Table134534610" displayName="Table134534610" ref="A9:E88" totalsRowShown="0" headerRowDxfId="25" dataDxfId="24">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="9" xr:uid="{25A0FEFF-9550-49E1-8274-9CC0D23D601A}" name="Table134534610" displayName="Table134534610" ref="A9:E88" totalsRowShown="0" headerRowDxfId="26" dataDxfId="25">
   <autoFilter ref="A9:E88" xr:uid="{25A0FEFF-9550-49E1-8274-9CC0D23D601A}"/>
   <tableColumns count="5">
-    <tableColumn id="1" xr3:uid="{4BCF3543-6F5A-4332-BFB4-BEC32B3DD532}" name="Code" dataDxfId="23"/>
-    <tableColumn id="2" xr3:uid="{6FA24118-5356-49C2-8800-833F470E365B}" name="Libellé niveau 1" dataDxfId="22"/>
-    <tableColumn id="5" xr3:uid="{AB6C4AE4-DA11-404C-A2AF-634EB6B21A48}" name="Libellé niveau 2" dataDxfId="21"/>
-    <tableColumn id="9" xr3:uid="{17784762-E727-4CE7-93CF-C096A4F54EC7}" name="Description" dataDxfId="20"/>
-    <tableColumn id="4" xr3:uid="{98D4AC23-8F15-4A2B-86D2-F4418A961F01}" name="Commentaire" dataDxfId="19"/>
+    <tableColumn id="1" xr3:uid="{4BCF3543-6F5A-4332-BFB4-BEC32B3DD532}" name="Code" dataDxfId="24"/>
+    <tableColumn id="2" xr3:uid="{6FA24118-5356-49C2-8800-833F470E365B}" name="Libellé niveau 1" dataDxfId="23"/>
+    <tableColumn id="5" xr3:uid="{AB6C4AE4-DA11-404C-A2AF-634EB6B21A48}" name="Libellé niveau 2" dataDxfId="22"/>
+    <tableColumn id="9" xr3:uid="{17784762-E727-4CE7-93CF-C096A4F54EC7}" name="Description" dataDxfId="21"/>
+    <tableColumn id="4" xr3:uid="{98D4AC23-8F15-4A2B-86D2-F4418A961F01}" name="Commentaire" dataDxfId="20"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -6400,12 +6400,12 @@
       <selection activeCell="A55" sqref="A55"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="26.140625" customWidth="1"/>
-    <col min="2" max="3" width="22.42578125" customWidth="1"/>
-    <col min="4" max="4" width="138.42578125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="26.140625" customWidth="1"/>
+    <col min="1" max="1" width="26.1640625" customWidth="1"/>
+    <col min="2" max="3" width="22.5" customWidth="1"/>
+    <col min="4" max="4" width="138.5" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="26.1640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5">
@@ -7531,12 +7531,12 @@
       <selection activeCell="A58" sqref="A58"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="26.140625" customWidth="1"/>
-    <col min="2" max="3" width="22.42578125" customWidth="1"/>
-    <col min="4" max="4" width="26.42578125" customWidth="1"/>
-    <col min="5" max="5" width="26.140625" customWidth="1"/>
+    <col min="1" max="1" width="26.1640625" customWidth="1"/>
+    <col min="2" max="3" width="22.5" customWidth="1"/>
+    <col min="4" max="4" width="26.5" customWidth="1"/>
+    <col min="5" max="5" width="26.1640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5">
@@ -8349,12 +8349,12 @@
       <selection activeCell="G16" sqref="G16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="26.140625" customWidth="1"/>
-    <col min="2" max="2" width="22.42578125" customWidth="1"/>
-    <col min="3" max="3" width="26.42578125" customWidth="1"/>
-    <col min="4" max="4" width="26.140625" customWidth="1"/>
+    <col min="1" max="1" width="26.1640625" customWidth="1"/>
+    <col min="2" max="2" width="22.5" customWidth="1"/>
+    <col min="3" max="3" width="26.5" customWidth="1"/>
+    <col min="4" max="4" width="26.1640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4">
@@ -8507,12 +8507,12 @@
       <selection activeCell="D16" sqref="D16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="26.140625" customWidth="1"/>
-    <col min="2" max="2" width="22.42578125" customWidth="1"/>
-    <col min="3" max="3" width="26.42578125" customWidth="1"/>
-    <col min="4" max="4" width="26.140625" customWidth="1"/>
+    <col min="1" max="1" width="26.1640625" customWidth="1"/>
+    <col min="2" max="2" width="22.5" customWidth="1"/>
+    <col min="3" max="3" width="26.5" customWidth="1"/>
+    <col min="4" max="4" width="26.1640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4">
@@ -8638,12 +8638,12 @@
       <selection activeCell="A164" sqref="A164"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="26.140625" customWidth="1"/>
-    <col min="2" max="4" width="22.42578125" customWidth="1"/>
-    <col min="5" max="6" width="26.42578125" customWidth="1"/>
-    <col min="7" max="7" width="26.140625" customWidth="1"/>
+    <col min="1" max="1" width="26.1640625" customWidth="1"/>
+    <col min="2" max="4" width="22.5" customWidth="1"/>
+    <col min="5" max="6" width="26.5" customWidth="1"/>
+    <col min="7" max="7" width="26.1640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6">
@@ -11323,16 +11323,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E30241F7-D304-4551-9EC7-136E462A509A}">
   <dimension ref="A1:E62"/>
   <sheetViews>
-    <sheetView topLeftCell="A45" workbookViewId="0">
-      <selection activeCell="A63" sqref="A63"/>
+    <sheetView tabSelected="1" topLeftCell="A45" workbookViewId="0">
+      <selection activeCell="E82" sqref="E82"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="26.140625" customWidth="1"/>
-    <col min="2" max="3" width="22.42578125" customWidth="1"/>
-    <col min="4" max="5" width="26.42578125" customWidth="1"/>
-    <col min="6" max="6" width="26.140625" customWidth="1"/>
+    <col min="1" max="1" width="26.1640625" customWidth="1"/>
+    <col min="2" max="3" width="22.5" customWidth="1"/>
+    <col min="4" max="5" width="26.5" customWidth="1"/>
+    <col min="6" max="6" width="26.1640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5">
@@ -12205,13 +12205,13 @@
       <selection activeCell="A26" sqref="A26"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="26.140625" customWidth="1"/>
-    <col min="2" max="3" width="22.42578125" customWidth="1"/>
-    <col min="4" max="4" width="63.28515625" customWidth="1"/>
-    <col min="5" max="5" width="26.42578125" customWidth="1"/>
-    <col min="6" max="6" width="26.140625" customWidth="1"/>
+    <col min="1" max="1" width="26.1640625" customWidth="1"/>
+    <col min="2" max="3" width="22.5" customWidth="1"/>
+    <col min="4" max="4" width="63.33203125" customWidth="1"/>
+    <col min="5" max="5" width="26.5" customWidth="1"/>
+    <col min="6" max="6" width="26.1640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5">
@@ -12560,16 +12560,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{92435A48-662D-466D-AB85-8A75AEE97CA6}">
   <dimension ref="A1:D30"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="O1" workbookViewId="0">
-      <selection activeCell="C24" sqref="C24"/>
+    <sheetView topLeftCell="A7" zoomScale="209" workbookViewId="0">
+      <selection activeCell="C17" sqref="C17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="26.140625" customWidth="1"/>
-    <col min="2" max="2" width="22.42578125" customWidth="1"/>
-    <col min="3" max="3" width="26.42578125" customWidth="1"/>
-    <col min="4" max="4" width="26.140625" customWidth="1"/>
+    <col min="1" max="1" width="26.1640625" customWidth="1"/>
+    <col min="2" max="2" width="22.5" customWidth="1"/>
+    <col min="3" max="3" width="26.5" customWidth="1"/>
+    <col min="4" max="4" width="26.1640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4">
@@ -12653,8 +12653,8 @@
       <c r="B10" s="7" t="s">
         <v>809</v>
       </c>
-      <c r="C10" s="8" t="s">
-        <v>810</v>
+      <c r="C10" s="7" t="s">
+        <v>809</v>
       </c>
       <c r="D10" s="8"/>
     </row>
@@ -12665,8 +12665,8 @@
       <c r="B11" s="7" t="s">
         <v>812</v>
       </c>
-      <c r="C11" s="8" t="s">
-        <v>813</v>
+      <c r="C11" s="7" t="s">
+        <v>812</v>
       </c>
       <c r="D11" s="8"/>
     </row>
@@ -12677,8 +12677,8 @@
       <c r="B12" s="7" t="s">
         <v>815</v>
       </c>
-      <c r="C12" s="8" t="s">
-        <v>816</v>
+      <c r="C12" s="7" t="s">
+        <v>815</v>
       </c>
       <c r="D12" s="8"/>
     </row>
@@ -12689,8 +12689,8 @@
       <c r="B13" s="7" t="s">
         <v>818</v>
       </c>
-      <c r="C13" s="9" t="s">
-        <v>819</v>
+      <c r="C13" s="7" t="s">
+        <v>818</v>
       </c>
       <c r="D13" s="9"/>
     </row>
@@ -12724,12 +12724,12 @@
       <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="26.140625" customWidth="1"/>
-    <col min="2" max="2" width="22.42578125" customWidth="1"/>
-    <col min="3" max="3" width="26.42578125" style="15" customWidth="1"/>
-    <col min="4" max="4" width="26.140625" customWidth="1"/>
+    <col min="1" max="1" width="26.1640625" customWidth="1"/>
+    <col min="2" max="2" width="22.5" customWidth="1"/>
+    <col min="3" max="3" width="26.5" style="15" customWidth="1"/>
+    <col min="4" max="4" width="26.1640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4">
@@ -12806,7 +12806,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="10" spans="1:4" ht="34.5">
+    <row r="10" spans="1:4" ht="37">
       <c r="A10" s="8">
         <v>1</v>
       </c>
@@ -12818,7 +12818,7 @@
       </c>
       <c r="D10" s="8"/>
     </row>
-    <row r="11" spans="1:4" ht="34.5">
+    <row r="11" spans="1:4" ht="37">
       <c r="A11" s="8">
         <v>2</v>
       </c>
@@ -12830,7 +12830,7 @@
       </c>
       <c r="D11" s="8"/>
     </row>
-    <row r="12" spans="1:4" ht="68.25">
+    <row r="12" spans="1:4" ht="61">
       <c r="A12" s="8">
         <v>3</v>
       </c>
@@ -12842,7 +12842,7 @@
       </c>
       <c r="D12" s="8"/>
     </row>
-    <row r="13" spans="1:4" ht="102">
+    <row r="13" spans="1:4" ht="85">
       <c r="A13" s="8">
         <v>4</v>
       </c>
@@ -12854,7 +12854,7 @@
       </c>
       <c r="D13" s="9"/>
     </row>
-    <row r="14" spans="1:4" ht="102">
+    <row r="14" spans="1:4" ht="85">
       <c r="A14" s="8">
         <v>5</v>
       </c>
@@ -12883,12 +12883,12 @@
       <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="26.140625" customWidth="1"/>
-    <col min="2" max="2" width="22.42578125" customWidth="1"/>
-    <col min="3" max="3" width="26.42578125" style="15" customWidth="1"/>
-    <col min="4" max="4" width="26.140625" customWidth="1"/>
+    <col min="1" max="1" width="26.1640625" customWidth="1"/>
+    <col min="2" max="2" width="22.5" customWidth="1"/>
+    <col min="3" max="3" width="26.5" style="15" customWidth="1"/>
+    <col min="4" max="4" width="26.1640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4">
@@ -12965,7 +12965,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="10" spans="1:4" ht="45.75">
+    <row r="10" spans="1:4" ht="49">
       <c r="A10" s="8" t="s">
         <v>832</v>
       </c>
@@ -12989,7 +12989,7 @@
       </c>
       <c r="D11" s="8"/>
     </row>
-    <row r="12" spans="1:4" ht="34.5">
+    <row r="12" spans="1:4" ht="25">
       <c r="A12" s="8" t="s">
         <v>836</v>
       </c>
@@ -13001,7 +13001,7 @@
       </c>
       <c r="D12" s="8"/>
     </row>
-    <row r="13" spans="1:4" ht="68.25">
+    <row r="13" spans="1:4" ht="61">
       <c r="A13" s="8" t="s">
         <v>838</v>
       </c>
@@ -13030,12 +13030,12 @@
       <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="26.140625" customWidth="1"/>
-    <col min="2" max="2" width="22.42578125" customWidth="1"/>
-    <col min="3" max="3" width="26.42578125" customWidth="1"/>
-    <col min="4" max="4" width="26.140625" customWidth="1"/>
+    <col min="1" max="1" width="26.1640625" customWidth="1"/>
+    <col min="2" max="2" width="22.5" customWidth="1"/>
+    <col min="3" max="3" width="26.5" customWidth="1"/>
+    <col min="4" max="4" width="26.1640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4">
@@ -13180,12 +13180,12 @@
       <selection activeCell="A89" sqref="A89"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="26.140625" customWidth="1"/>
-    <col min="2" max="3" width="22.42578125" customWidth="1"/>
-    <col min="4" max="5" width="26.42578125" customWidth="1"/>
-    <col min="6" max="6" width="26.140625" customWidth="1"/>
+    <col min="1" max="1" width="26.1640625" customWidth="1"/>
+    <col min="2" max="3" width="22.5" customWidth="1"/>
+    <col min="4" max="5" width="26.5" customWidth="1"/>
+    <col min="6" max="6" width="26.1640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5">
@@ -14451,17 +14451,8 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document - Suivi de projet" ma:contentTypeID="0x010100333226B5D6902549BFE4A72F45A4400B0100E98F8C089710A74CA077FC6D601326A8" ma:contentTypeVersion="51" ma:contentTypeDescription="Type de contenu - Documentation de suivi de projet" ma:contentTypeScope="" ma:versionID="5f25723db95d46bd813c254178c12b28">
-  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns1="http://schemas.microsoft.com/sharepoint/v3" xmlns:ns2="f6ca01e7-bd19-41f1-999c-e032ef5104c3" xmlns:ns3="1720d4e8-2b1e-4bd1-aad5-1b4debf9b56d" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="7bc30f4eda6069462a66ebc021061e28" ns1:_="" ns2:_="" ns3:_="">
+<ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document - Suivi de projet" ma:contentTypeID="0x010100333226B5D6902549BFE4A72F45A4400B0100E98F8C089710A74CA077FC6D601326A8" ma:contentTypeVersion="51" ma:contentTypeDescription="Type de contenu - Documentation de suivi de projet" ma:contentTypeScope="" ma:versionID="8bde4621cafd3c37adf5055c98b7a9b0">
+  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns1="http://schemas.microsoft.com/sharepoint/v3" xmlns:ns2="f6ca01e7-bd19-41f1-999c-e032ef5104c3" xmlns:ns3="1720d4e8-2b1e-4bd1-aad5-1b4debf9b56d" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="351baf626036704bc2f52fdf6ad997bc" ns1:_="" ns2:_="" ns3:_="">
     <xsd:import namespace="http://schemas.microsoft.com/sharepoint/v3"/>
     <xsd:import namespace="f6ca01e7-bd19-41f1-999c-e032ef5104c3"/>
     <xsd:import namespace="1720d4e8-2b1e-4bd1-aad5-1b4debf9b56d"/>
@@ -14523,12 +14514,12 @@
         </xsd:restriction>
       </xsd:simpleType>
     </xsd:element>
-    <xsd:element name="_ip_UnifiedCompliancePolicyProperties" ma:index="49" nillable="true" ma:displayName="Propriétés de la stratégie de conformité unifiée" ma:hidden="true" ma:internalName="_ip_UnifiedCompliancePolicyProperties">
+    <xsd:element name="_ip_UnifiedCompliancePolicyProperties" ma:index="49" nillable="true" ma:displayName="Unified Compliance Policy Properties" ma:hidden="true" ma:internalName="_ip_UnifiedCompliancePolicyProperties">
       <xsd:simpleType>
         <xsd:restriction base="dms:Note"/>
       </xsd:simpleType>
     </xsd:element>
-    <xsd:element name="_ip_UnifiedCompliancePolicyUIAction" ma:index="50" nillable="true" ma:displayName="Action d’interface utilisateur de la stratégie de conformité unifiée" ma:hidden="true" ma:internalName="_ip_UnifiedCompliancePolicyUIAction">
+    <xsd:element name="_ip_UnifiedCompliancePolicyUIAction" ma:index="50" nillable="true" ma:displayName="Unified Compliance Policy UI Action" ma:hidden="true" ma:internalName="_ip_UnifiedCompliancePolicyUIAction">
       <xsd:simpleType>
         <xsd:restriction base="dms:Text"/>
       </xsd:simpleType>
@@ -14641,7 +14632,7 @@
         </xsd:restriction>
       </xsd:simpleType>
     </xsd:element>
-    <xsd:element name="SharedWithUsers" ma:index="35" nillable="true" ma:displayName="Partagé avec" ma:internalName="SharedWithUsers" ma:readOnly="true">
+    <xsd:element name="SharedWithUsers" ma:index="35" nillable="true" ma:displayName="Shared With" ma:internalName="SharedWithUsers" ma:readOnly="true">
       <xsd:complexType>
         <xsd:complexContent>
           <xsd:extension base="dms:UserMulti">
@@ -14660,7 +14651,7 @@
         </xsd:complexContent>
       </xsd:complexType>
     </xsd:element>
-    <xsd:element name="SharedWithDetails" ma:index="36" nillable="true" ma:displayName="Partagé avec détails" ma:internalName="SharedWithDetails" ma:readOnly="true">
+    <xsd:element name="SharedWithDetails" ma:index="36" nillable="true" ma:displayName="Shared With Details" ma:internalName="SharedWithDetails" ma:readOnly="true">
       <xsd:simpleType>
         <xsd:restriction base="dms:Note">
           <xsd:maxLength value="255"/>
@@ -14733,7 +14724,7 @@
         <xsd:restriction base="dms:Unknown"/>
       </xsd:simpleType>
     </xsd:element>
-    <xsd:element name="lcf76f155ced4ddcb4097134ff3c332f" ma:index="44" nillable="true" ma:taxonomy="true" ma:internalName="lcf76f155ced4ddcb4097134ff3c332f" ma:taxonomyFieldName="MediaServiceImageTags" ma:displayName="Balises d’images" ma:readOnly="false" ma:fieldId="{5cf76f15-5ced-4ddc-b409-7134ff3c332f}" ma:taxonomyMulti="true" ma:sspId="c4480557-28ee-4200-b705-f4b4ceb9c11a" ma:termSetId="09814cd3-568e-fe90-9814-8d621ff8fb84" ma:anchorId="fba54fb3-c3e1-fe81-a776-ca4b69148c4d" ma:open="true" ma:isKeyword="false">
+    <xsd:element name="lcf76f155ced4ddcb4097134ff3c332f" ma:index="44" nillable="true" ma:taxonomy="true" ma:internalName="lcf76f155ced4ddcb4097134ff3c332f" ma:taxonomyFieldName="MediaServiceImageTags" ma:displayName="Image Tags" ma:readOnly="false" ma:fieldId="{5cf76f15-5ced-4ddc-b409-7134ff3c332f}" ma:taxonomyMulti="true" ma:sspId="c4480557-28ee-4200-b705-f4b4ceb9c11a" ma:termSetId="09814cd3-568e-fe90-9814-8d621ff8fb84" ma:anchorId="fba54fb3-c3e1-fe81-a776-ca4b69148c4d" ma:open="true" ma:isKeyword="false">
       <xsd:complexType>
         <xsd:sequence>
           <xsd:element ref="pc:Terms" minOccurs="0" maxOccurs="1"/>
@@ -14777,8 +14768,8 @@
         <xsd:element ref="dc:creator" minOccurs="0" maxOccurs="1"/>
         <xsd:element ref="dcterms:created" minOccurs="0" maxOccurs="1"/>
         <xsd:element ref="dc:identifier" minOccurs="0" maxOccurs="1"/>
-        <xsd:element name="contentType" minOccurs="0" maxOccurs="1" type="xsd:string" ma:index="7" ma:displayName="Type de contenu"/>
-        <xsd:element ref="dc:title" minOccurs="0" maxOccurs="1" ma:index="1" ma:displayName="Titre"/>
+        <xsd:element name="contentType" minOccurs="0" maxOccurs="1" type="xsd:string" ma:index="7" ma:displayName="Content Type"/>
+        <xsd:element ref="dc:title" minOccurs="0" maxOccurs="1" ma:index="1" ma:displayName="Title"/>
         <xsd:element ref="dc:subject" minOccurs="0" maxOccurs="1"/>
         <xsd:element ref="dc:description" minOccurs="0" maxOccurs="1"/>
         <xsd:element name="keywords" minOccurs="0" maxOccurs="1" type="xsd:string"/>
@@ -14867,10 +14858,23 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C5967638-FCD9-44FD-B4E1-300D2A834C2B}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{FC9CF232-17D3-4121-B9E8-F29E5F166866}"/>
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{CD036102-29D9-4EAA-A051-1584354EFFAD}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C5967638-FCD9-44FD-B4E1-300D2A834C2B}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
[23.12.01 17:53] Model auto-generation
</commit_message>
<xml_diff>
--- a/nomenclature_parser/in/Nomenclatures EMSI EVENT.xlsx
+++ b/nomenclature_parser/in/Nomenclatures EMSI EVENT.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://esantegouv.sharepoint.com/sites/GED-Calypso/espace-projets/Espace Programme SISAMU/01 - Equipe projet/07 - Innovation et prospectif/12 - Hub Santé/17 - MDD/Nomenclatures/01 - Base interne/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="884" documentId="13_ncr:1_{420DE2DB-F177-420D-9F91-385C2DF0C062}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{C536996A-4D50-FC45-90DD-15C8F77C2A33}"/>
+  <xr:revisionPtr revIDLastSave="885" documentId="13_ncr:1_{420DE2DB-F177-420D-9F91-385C2DF0C062}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{D361D6F6-62B4-AC4D-9E90-7339E4425E85}"/>
   <bookViews>
-    <workbookView xWindow="2680" yWindow="-20640" windowWidth="34560" windowHeight="20160" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="-20640" windowWidth="34560" windowHeight="20160" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="EVENT.ETYPE.CATEGORY" sheetId="9" r:id="rId1"/>
@@ -38,8 +38,6 @@
         <xcalcf:feature name="microsoft.com:FV"/>
         <xcalcf:feature name="microsoft.com:CNMTM"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -47,7 +45,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1950" uniqueCount="1236">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1950" uniqueCount="1237">
   <si>
     <t>Référentiel nomenclature</t>
   </si>
@@ -3755,6 +3753,9 @@
   </si>
   <si>
     <t>Naturel</t>
+  </si>
+  <si>
+    <t>ANIMAUX</t>
   </si>
 </sst>
 </file>
@@ -3935,41 +3936,6 @@
     <cellStyle name="Normal 2" xfId="2" xr:uid="{289B6461-38A1-47EB-AD2F-3A7ED8C77D6E}"/>
   </cellStyles>
   <dxfs count="79">
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="8"/>
-        <color auto="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
     <dxf>
       <font>
         <b val="0"/>
@@ -5188,6 +5154,41 @@
         <family val="2"/>
         <scheme val="minor"/>
       </font>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="8"/>
+        <color auto="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
       <border diagonalUp="0" diagonalDown="0">
         <left style="thin">
           <color indexed="64"/>
@@ -5983,40 +5984,40 @@
 </file>
 
 <file path=xl/tables/table10.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="12" xr:uid="{26DF3307-34F4-42AE-84A4-0D4CBF066D54}" name="Table134579111213" displayName="Table134579111213" ref="A9:E57" totalsRowShown="0" headerRowDxfId="19" dataDxfId="18">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="12" xr:uid="{26DF3307-34F4-42AE-84A4-0D4CBF066D54}" name="Table134579111213" displayName="Table134579111213" ref="A9:E57" totalsRowShown="0" headerRowDxfId="18" dataDxfId="17">
   <autoFilter ref="A9:E57" xr:uid="{B3C2A837-EDE7-4BB4-94EB-1FCD3E6C6353}"/>
   <tableColumns count="5">
-    <tableColumn id="1" xr3:uid="{26EE7CCE-0A08-4908-A677-59C683486D38}" name="Code" dataDxfId="17"/>
-    <tableColumn id="2" xr3:uid="{CDC16B11-DD37-446F-8F21-E3D9026DD97C}" name="Libellé niveau 1" dataDxfId="16"/>
-    <tableColumn id="5" xr3:uid="{A51DB763-9299-451D-A810-BCEA65D9E01D}" name="Libellé niveau 2" dataDxfId="15"/>
-    <tableColumn id="3" xr3:uid="{A4FF1C94-E2C0-4BEC-A828-8B7732E4CD60}" name="Description" dataDxfId="14"/>
-    <tableColumn id="4" xr3:uid="{C1E7BA75-D90A-44E9-823B-A6443FBAB216}" name="Commentaire" dataDxfId="13"/>
+    <tableColumn id="1" xr3:uid="{26EE7CCE-0A08-4908-A677-59C683486D38}" name="Code" dataDxfId="16"/>
+    <tableColumn id="2" xr3:uid="{CDC16B11-DD37-446F-8F21-E3D9026DD97C}" name="Libellé niveau 1" dataDxfId="15"/>
+    <tableColumn id="5" xr3:uid="{A51DB763-9299-451D-A810-BCEA65D9E01D}" name="Libellé niveau 2" dataDxfId="14"/>
+    <tableColumn id="3" xr3:uid="{A4FF1C94-E2C0-4BEC-A828-8B7732E4CD60}" name="Description" dataDxfId="13"/>
+    <tableColumn id="4" xr3:uid="{C1E7BA75-D90A-44E9-823B-A6443FBAB216}" name="Commentaire" dataDxfId="12"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table11.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="10" xr:uid="{CDF36831-79C4-46E2-A8A4-A2D002055482}" name="Table13457911" displayName="Table13457911" ref="A9:D15" totalsRowShown="0" headerRowDxfId="12" dataDxfId="11">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="10" xr:uid="{CDF36831-79C4-46E2-A8A4-A2D002055482}" name="Table13457911" displayName="Table13457911" ref="A9:D15" totalsRowShown="0" headerRowDxfId="11" dataDxfId="10">
   <autoFilter ref="A9:D15" xr:uid="{CDF36831-79C4-46E2-A8A4-A2D002055482}"/>
   <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{827CD47C-54B9-492C-BEC1-38B3CBDEA92E}" name="Code" dataDxfId="10"/>
-    <tableColumn id="2" xr3:uid="{B7ADDE36-930D-429D-B06C-F6B843153C60}" name="Libellé niveau 1" dataDxfId="9"/>
-    <tableColumn id="3" xr3:uid="{DB478352-58AC-4CF9-AEB7-17CD612D9C64}" name="Description" dataDxfId="8"/>
-    <tableColumn id="4" xr3:uid="{63664487-54C4-4FB8-9A75-EE1F75C736C2}" name="Commentaire" dataDxfId="7"/>
+    <tableColumn id="1" xr3:uid="{827CD47C-54B9-492C-BEC1-38B3CBDEA92E}" name="Code" dataDxfId="9"/>
+    <tableColumn id="2" xr3:uid="{B7ADDE36-930D-429D-B06C-F6B843153C60}" name="Libellé niveau 1" dataDxfId="8"/>
+    <tableColumn id="3" xr3:uid="{DB478352-58AC-4CF9-AEB7-17CD612D9C64}" name="Description" dataDxfId="7"/>
+    <tableColumn id="4" xr3:uid="{63664487-54C4-4FB8-9A75-EE1F75C736C2}" name="Commentaire" dataDxfId="6"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table12.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="11" xr:uid="{B3C2A837-EDE7-4BB4-94EB-1FCD3E6C6353}" name="Table1345791112" displayName="Table1345791112" ref="A9:D12" totalsRowShown="0" headerRowDxfId="6" dataDxfId="5">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="11" xr:uid="{B3C2A837-EDE7-4BB4-94EB-1FCD3E6C6353}" name="Table1345791112" displayName="Table1345791112" ref="A9:D12" totalsRowShown="0" headerRowDxfId="5" dataDxfId="4">
   <autoFilter ref="A9:D12" xr:uid="{B3C2A837-EDE7-4BB4-94EB-1FCD3E6C6353}"/>
   <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{FF144121-7487-4B50-8A65-49A8AC28EBBC}" name="Code" dataDxfId="4"/>
-    <tableColumn id="2" xr3:uid="{419998F0-6C22-4337-887A-52DAD4433A40}" name="Libellé niveau 1" dataDxfId="3"/>
-    <tableColumn id="3" xr3:uid="{30E5AAA1-E57D-4F0A-AE50-7AE2BAEBE289}" name="Description" dataDxfId="2"/>
-    <tableColumn id="4" xr3:uid="{4BFF9456-387C-4FEC-94E6-13FEF83002CF}" name="Commentaire" dataDxfId="1"/>
+    <tableColumn id="1" xr3:uid="{FF144121-7487-4B50-8A65-49A8AC28EBBC}" name="Code" dataDxfId="3"/>
+    <tableColumn id="2" xr3:uid="{419998F0-6C22-4337-887A-52DAD4433A40}" name="Libellé niveau 1" dataDxfId="2"/>
+    <tableColumn id="3" xr3:uid="{30E5AAA1-E57D-4F0A-AE50-7AE2BAEBE289}" name="Description" dataDxfId="1"/>
+    <tableColumn id="4" xr3:uid="{4BFF9456-387C-4FEC-94E6-13FEF83002CF}" name="Commentaire" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -6071,61 +6072,61 @@
   <tableColumns count="4">
     <tableColumn id="1" xr3:uid="{5F5C37BB-9414-45F4-882F-C30DBF6693A5}" name="Code" dataDxfId="47"/>
     <tableColumn id="2" xr3:uid="{8CC3DA00-B777-4A14-9918-8E544FEE762C}" name="Libellé niveau 1" dataDxfId="46"/>
-    <tableColumn id="3" xr3:uid="{22407615-9D4D-48D6-B548-25DBB05445D9}" name="Description" dataDxfId="0"/>
-    <tableColumn id="4" xr3:uid="{457E12C2-4B88-45D4-BB7E-F312B1CD816C}" name="Commentaire" dataDxfId="45"/>
+    <tableColumn id="3" xr3:uid="{22407615-9D4D-48D6-B548-25DBB05445D9}" name="Description" dataDxfId="45"/>
+    <tableColumn id="4" xr3:uid="{457E12C2-4B88-45D4-BB7E-F312B1CD816C}" name="Commentaire" dataDxfId="44"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="7" xr:uid="{1BA9C99E-0FEA-4661-A32A-C70E83B4A5DF}" name="Table134578" displayName="Table134578" ref="A9:D14" totalsRowShown="0" headerRowDxfId="44" dataDxfId="43">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="7" xr:uid="{1BA9C99E-0FEA-4661-A32A-C70E83B4A5DF}" name="Table134578" displayName="Table134578" ref="A9:D14" totalsRowShown="0" headerRowDxfId="43" dataDxfId="42">
   <autoFilter ref="A9:D14" xr:uid="{1BA9C99E-0FEA-4661-A32A-C70E83B4A5DF}"/>
   <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{5D7488F6-CDA9-48C2-A99F-2DE474359121}" name="Code" dataDxfId="42"/>
-    <tableColumn id="2" xr3:uid="{AE5DDD33-6682-42EF-85AC-99A3CAC427CE}" name="Libellé niveau 1" dataDxfId="41"/>
-    <tableColumn id="3" xr3:uid="{BE555B52-6698-4900-A795-2697B7BF98AE}" name="Description" dataDxfId="40"/>
-    <tableColumn id="4" xr3:uid="{FBA181AC-8F3F-4A9C-9A04-E19FDB35DE0E}" name="Commentaire" dataDxfId="39"/>
+    <tableColumn id="1" xr3:uid="{5D7488F6-CDA9-48C2-A99F-2DE474359121}" name="Code" dataDxfId="41"/>
+    <tableColumn id="2" xr3:uid="{AE5DDD33-6682-42EF-85AC-99A3CAC427CE}" name="Libellé niveau 1" dataDxfId="40"/>
+    <tableColumn id="3" xr3:uid="{BE555B52-6698-4900-A795-2697B7BF98AE}" name="Description" dataDxfId="39"/>
+    <tableColumn id="4" xr3:uid="{FBA181AC-8F3F-4A9C-9A04-E19FDB35DE0E}" name="Commentaire" dataDxfId="38"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table7.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{9BBAEC71-98FF-4AB8-B5E1-1CE8C8584409}" name="Table1345" displayName="Table1345" ref="A9:D13" totalsRowShown="0" headerRowDxfId="38" dataDxfId="37">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{9BBAEC71-98FF-4AB8-B5E1-1CE8C8584409}" name="Table1345" displayName="Table1345" ref="A9:D13" totalsRowShown="0" headerRowDxfId="37" dataDxfId="36">
   <autoFilter ref="A9:D13" xr:uid="{9BBAEC71-98FF-4AB8-B5E1-1CE8C8584409}"/>
   <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{CC3785D5-DB9A-4D60-862F-F8E090985E56}" name="Code" dataDxfId="36"/>
-    <tableColumn id="2" xr3:uid="{0E29D007-DD2B-4361-B0B6-3124B15DD8DA}" name="Libellé niveau 1" dataDxfId="35"/>
-    <tableColumn id="3" xr3:uid="{2F058103-5AD9-4F2B-A662-54DD0A6EEAE9}" name="Description" dataDxfId="34"/>
-    <tableColumn id="4" xr3:uid="{E9F88BD4-157D-4840-B9EE-0122B96E7D08}" name="Commentaire" dataDxfId="33"/>
+    <tableColumn id="1" xr3:uid="{CC3785D5-DB9A-4D60-862F-F8E090985E56}" name="Code" dataDxfId="35"/>
+    <tableColumn id="2" xr3:uid="{0E29D007-DD2B-4361-B0B6-3124B15DD8DA}" name="Libellé niveau 1" dataDxfId="34"/>
+    <tableColumn id="3" xr3:uid="{2F058103-5AD9-4F2B-A662-54DD0A6EEAE9}" name="Description" dataDxfId="33"/>
+    <tableColumn id="4" xr3:uid="{E9F88BD4-157D-4840-B9EE-0122B96E7D08}" name="Commentaire" dataDxfId="32"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table8.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="8" xr:uid="{448164F5-1D63-43E2-8F84-C919457EC610}" name="Table134579" displayName="Table134579" ref="A9:D12" totalsRowShown="0" headerRowDxfId="32" dataDxfId="31">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="8" xr:uid="{448164F5-1D63-43E2-8F84-C919457EC610}" name="Table134579" displayName="Table134579" ref="A9:D12" totalsRowShown="0" headerRowDxfId="31" dataDxfId="30">
   <autoFilter ref="A9:D12" xr:uid="{448164F5-1D63-43E2-8F84-C919457EC610}"/>
   <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{033E47FB-ADF9-40CF-A20D-BF29E04ADB55}" name="Code" dataDxfId="30"/>
-    <tableColumn id="2" xr3:uid="{E55A0DD3-BD4F-4DD2-A60D-BB8F4A8862C6}" name="Libellé niveau 1" dataDxfId="29"/>
-    <tableColumn id="3" xr3:uid="{9682D9C0-6A4A-45B9-BAFE-9ADE23B9A964}" name="Description" dataDxfId="28"/>
-    <tableColumn id="4" xr3:uid="{6EDEDC97-62DF-432C-8466-D8B59200DD75}" name="Commentaire" dataDxfId="27"/>
+    <tableColumn id="1" xr3:uid="{033E47FB-ADF9-40CF-A20D-BF29E04ADB55}" name="Code" dataDxfId="29"/>
+    <tableColumn id="2" xr3:uid="{E55A0DD3-BD4F-4DD2-A60D-BB8F4A8862C6}" name="Libellé niveau 1" dataDxfId="28"/>
+    <tableColumn id="3" xr3:uid="{9682D9C0-6A4A-45B9-BAFE-9ADE23B9A964}" name="Description" dataDxfId="27"/>
+    <tableColumn id="4" xr3:uid="{6EDEDC97-62DF-432C-8466-D8B59200DD75}" name="Commentaire" dataDxfId="26"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table9.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="9" xr:uid="{25A0FEFF-9550-49E1-8274-9CC0D23D601A}" name="Table134534610" displayName="Table134534610" ref="A9:E88" totalsRowShown="0" headerRowDxfId="26" dataDxfId="25">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="9" xr:uid="{25A0FEFF-9550-49E1-8274-9CC0D23D601A}" name="Table134534610" displayName="Table134534610" ref="A9:E88" totalsRowShown="0" headerRowDxfId="25" dataDxfId="24">
   <autoFilter ref="A9:E88" xr:uid="{25A0FEFF-9550-49E1-8274-9CC0D23D601A}"/>
   <tableColumns count="5">
-    <tableColumn id="1" xr3:uid="{4BCF3543-6F5A-4332-BFB4-BEC32B3DD532}" name="Code" dataDxfId="24"/>
-    <tableColumn id="2" xr3:uid="{6FA24118-5356-49C2-8800-833F470E365B}" name="Libellé niveau 1" dataDxfId="23"/>
-    <tableColumn id="5" xr3:uid="{AB6C4AE4-DA11-404C-A2AF-634EB6B21A48}" name="Libellé niveau 2" dataDxfId="22"/>
-    <tableColumn id="9" xr3:uid="{17784762-E727-4CE7-93CF-C096A4F54EC7}" name="Description" dataDxfId="21"/>
-    <tableColumn id="4" xr3:uid="{98D4AC23-8F15-4A2B-86D2-F4418A961F01}" name="Commentaire" dataDxfId="20"/>
+    <tableColumn id="1" xr3:uid="{4BCF3543-6F5A-4332-BFB4-BEC32B3DD532}" name="Code" dataDxfId="23"/>
+    <tableColumn id="2" xr3:uid="{6FA24118-5356-49C2-8800-833F470E365B}" name="Libellé niveau 1" dataDxfId="22"/>
+    <tableColumn id="5" xr3:uid="{AB6C4AE4-DA11-404C-A2AF-634EB6B21A48}" name="Libellé niveau 2" dataDxfId="21"/>
+    <tableColumn id="9" xr3:uid="{17784762-E727-4CE7-93CF-C096A4F54EC7}" name="Description" dataDxfId="20"/>
+    <tableColumn id="4" xr3:uid="{98D4AC23-8F15-4A2B-86D2-F4418A961F01}" name="Commentaire" dataDxfId="19"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -8634,8 +8635,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B92BE96A-EA9D-4CCB-987C-51DCC55ED9E4}">
   <dimension ref="A1:F163"/>
   <sheetViews>
-    <sheetView topLeftCell="A95" workbookViewId="0">
-      <selection activeCell="A164" sqref="A164"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="15"/>
@@ -8747,7 +8748,7 @@
         <v>219</v>
       </c>
       <c r="B10" s="7" t="s">
-        <v>220</v>
+        <v>1236</v>
       </c>
       <c r="C10" s="8"/>
       <c r="D10" s="8"/>
@@ -11323,8 +11324,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E30241F7-D304-4551-9EC7-136E462A509A}">
   <dimension ref="A1:E62"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A45" workbookViewId="0">
-      <selection activeCell="E82" sqref="E82"/>
+    <sheetView topLeftCell="A45" workbookViewId="0">
+      <selection activeCell="C56" sqref="C56"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="15"/>
@@ -14451,6 +14452,15 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document - Suivi de projet" ma:contentTypeID="0x010100333226B5D6902549BFE4A72F45A4400B0100E98F8C089710A74CA077FC6D601326A8" ma:contentTypeVersion="51" ma:contentTypeDescription="Type de contenu - Documentation de suivi de projet" ma:contentTypeScope="" ma:versionID="8bde4621cafd3c37adf5055c98b7a9b0">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns1="http://schemas.microsoft.com/sharepoint/v3" xmlns:ns2="f6ca01e7-bd19-41f1-999c-e032ef5104c3" xmlns:ns3="1720d4e8-2b1e-4bd1-aad5-1b4debf9b56d" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="351baf626036704bc2f52fdf6ad997bc" ns1:_="" ns2:_="" ns3:_="">
     <xsd:import namespace="http://schemas.microsoft.com/sharepoint/v3"/>
@@ -14858,23 +14868,30 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{FC9CF232-17D3-4121-B9E8-F29E5F166866}"/>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C5967638-FCD9-44FD-B4E1-300D2A834C2B}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{FC9CF232-17D3-4121-B9E8-F29E5F166866}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
+    <ds:schemaRef ds:uri="f6ca01e7-bd19-41f1-999c-e032ef5104c3"/>
+    <ds:schemaRef ds:uri="1720d4e8-2b1e-4bd1-aad5-1b4debf9b56d"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
[23.12.01 17:58] Model auto-generation
</commit_message>
<xml_diff>
--- a/nomenclature_parser/in/Nomenclatures EMSI EVENT.xlsx
+++ b/nomenclature_parser/in/Nomenclatures EMSI EVENT.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://esantegouv.sharepoint.com/sites/GED-Calypso/espace-projets/Espace Programme SISAMU/01 - Equipe projet/07 - Innovation et prospectif/12 - Hub Santé/17 - MDD/Nomenclatures/01 - Base interne/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="885" documentId="13_ncr:1_{420DE2DB-F177-420D-9F91-385C2DF0C062}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{D361D6F6-62B4-AC4D-9E90-7339E4425E85}"/>
+  <xr:revisionPtr revIDLastSave="886" documentId="13_ncr:1_{420DE2DB-F177-420D-9F91-385C2DF0C062}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{9C47E026-8F30-0548-8819-BB7858245045}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="-20640" windowWidth="34560" windowHeight="20160" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -45,7 +45,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1950" uniqueCount="1237">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1950" uniqueCount="1236">
   <si>
     <t>Référentiel nomenclature</t>
   </si>
@@ -3753,9 +3753,6 @@
   </si>
   <si>
     <t>Naturel</t>
-  </si>
-  <si>
-    <t>ANIMAUX</t>
   </si>
 </sst>
 </file>
@@ -8636,7 +8633,7 @@
   <dimension ref="A1:F163"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="15"/>
@@ -8748,7 +8745,7 @@
         <v>219</v>
       </c>
       <c r="B10" s="7" t="s">
-        <v>1236</v>
+        <v>220</v>
       </c>
       <c r="C10" s="8"/>
       <c r="D10" s="8"/>

</xml_diff>

<commit_message>
[23.12.01 18:46] Model auto-generation
</commit_message>
<xml_diff>
--- a/nomenclature_parser/in/Nomenclatures EMSI EVENT.xlsx
+++ b/nomenclature_parser/in/Nomenclatures EMSI EVENT.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://esantegouv.sharepoint.com/sites/GED-Calypso/espace-projets/Espace Programme SISAMU/01 - Equipe projet/07 - Innovation et prospectif/12 - Hub Santé/17 - MDD/Nomenclatures/01 - Base interne/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="886" documentId="13_ncr:1_{420DE2DB-F177-420D-9F91-385C2DF0C062}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{9C47E026-8F30-0548-8819-BB7858245045}"/>
+  <xr:revisionPtr revIDLastSave="888" documentId="13_ncr:1_{420DE2DB-F177-420D-9F91-385C2DF0C062}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{DCFA4B39-A0D9-A04B-B72B-ABB69C273E31}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="-20640" windowWidth="34560" windowHeight="20160" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -14449,15 +14449,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document - Suivi de projet" ma:contentTypeID="0x010100333226B5D6902549BFE4A72F45A4400B0100E98F8C089710A74CA077FC6D601326A8" ma:contentTypeVersion="51" ma:contentTypeDescription="Type de contenu - Documentation de suivi de projet" ma:contentTypeScope="" ma:versionID="8bde4621cafd3c37adf5055c98b7a9b0">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns1="http://schemas.microsoft.com/sharepoint/v3" xmlns:ns2="f6ca01e7-bd19-41f1-999c-e032ef5104c3" xmlns:ns3="1720d4e8-2b1e-4bd1-aad5-1b4debf9b56d" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="351baf626036704bc2f52fdf6ad997bc" ns1:_="" ns2:_="" ns3:_="">
     <xsd:import namespace="http://schemas.microsoft.com/sharepoint/v3"/>
@@ -14865,15 +14856,16 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C5967638-FCD9-44FD-B4E1-300D2A834C2B}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{FC9CF232-17D3-4121-B9E8-F29E5F166866}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -14891,4 +14883,12 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C5967638-FCD9-44FD-B4E1-300D2A834C2B}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
[23.12.01 18:54] Model auto-generation
</commit_message>
<xml_diff>
--- a/nomenclature_parser/in/Nomenclatures EMSI EVENT.xlsx
+++ b/nomenclature_parser/in/Nomenclatures EMSI EVENT.xlsx
@@ -8633,7 +8633,7 @@
   <dimension ref="A1:F163"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="15"/>
@@ -14449,6 +14449,15 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document - Suivi de projet" ma:contentTypeID="0x010100333226B5D6902549BFE4A72F45A4400B0100E98F8C089710A74CA077FC6D601326A8" ma:contentTypeVersion="51" ma:contentTypeDescription="Type de contenu - Documentation de suivi de projet" ma:contentTypeScope="" ma:versionID="8bde4621cafd3c37adf5055c98b7a9b0">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns1="http://schemas.microsoft.com/sharepoint/v3" xmlns:ns2="f6ca01e7-bd19-41f1-999c-e032ef5104c3" xmlns:ns3="1720d4e8-2b1e-4bd1-aad5-1b4debf9b56d" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="351baf626036704bc2f52fdf6ad997bc" ns1:_="" ns2:_="" ns3:_="">
     <xsd:import namespace="http://schemas.microsoft.com/sharepoint/v3"/>
@@ -14856,16 +14865,15 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C5967638-FCD9-44FD-B4E1-300D2A834C2B}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{FC9CF232-17D3-4121-B9E8-F29E5F166866}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -14883,12 +14891,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C5967638-FCD9-44FD-B4E1-300D2A834C2B}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
[24.11.25 17:41] Model auto-generation
</commit_message>
<xml_diff>
--- a/nomenclature_parser/in/Nomenclatures EMSI EVENT.xlsx
+++ b/nomenclature_parser/in/Nomenclatures EMSI EVENT.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="11010"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="11110"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://esantegouv.sharepoint.com/sites/GED-Calypso/espace-projets/Espace Programme SISAMU/01 - Equipe projet/07 - Innovation et prospectif/12 - Hub Santé/17 - MDD/Nomenclatures/01 - Base interne/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="888" documentId="13_ncr:1_{420DE2DB-F177-420D-9F91-385C2DF0C062}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{DCFA4B39-A0D9-A04B-B72B-ABB69C273E31}"/>
+  <xr:revisionPtr revIDLastSave="890" documentId="13_ncr:1_{420DE2DB-F177-420D-9F91-385C2DF0C062}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{E0D20EFD-A435-4E47-B5E9-04E3CE11D882}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="-20640" windowWidth="34560" windowHeight="20160" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -8633,7 +8633,7 @@
   <dimension ref="A1:F163"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+      <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="15"/>
@@ -14449,12 +14449,55 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <ModificateurAlfresco xmlns="f6ca01e7-bd19-41f1-999c-e032ef5104c3" xsi:nil="true"/>
+    <_ip_UnifiedCompliancePolicyUIAction xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+    <f8b6baa267c0456bbf6a8d18c49a130b xmlns="f6ca01e7-bd19-41f1-999c-e032ef5104c3">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </f8b6baa267c0456bbf6a8d18c49a130b>
+    <eef0f6fc4ed046399a9d01fd3a7d6a6a xmlns="f6ca01e7-bd19-41f1-999c-e032ef5104c3">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </eef0f6fc4ed046399a9d01fd3a7d6a6a>
+    <Référence_x0020_Bon_x0020_de_x0020_Commande xmlns="f6ca01e7-bd19-41f1-999c-e032ef5104c3" xsi:nil="true"/>
+    <Référence_x0020_Documentaire xmlns="f6ca01e7-bd19-41f1-999c-e032ef5104c3" xsi:nil="true"/>
+    <Chantier xmlns="f6ca01e7-bd19-41f1-999c-e032ef5104c3" xsi:nil="true"/>
+    <p671c8df16a44846939d278d4958f62c xmlns="f6ca01e7-bd19-41f1-999c-e032ef5104c3">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </p671c8df16a44846939d278d4958f62c>
+    <Durée_x0020_d_x0027_Utilité_x0020_Administrative_x0020__x0028_DUA_x0029_ xmlns="f6ca01e7-bd19-41f1-999c-e032ef5104c3" xsi:nil="true"/>
+    <Environnement xmlns="f6ca01e7-bd19-41f1-999c-e032ef5104c3" xsi:nil="true"/>
+    <b2804ef99be44b9e8166e80a6c2eb9f1 xmlns="f6ca01e7-bd19-41f1-999c-e032ef5104c3">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </b2804ef99be44b9e8166e80a6c2eb9f1>
+    <_ExtendedDescription xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+    <mc4aa6e782e045f6bb87dab01c971b56 xmlns="f6ca01e7-bd19-41f1-999c-e032ef5104c3">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </mc4aa6e782e045f6bb87dab01c971b56>
+    <_ip_UnifiedCompliancePolicyProperties xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+    <m312bc62cb0243b6a873cbbf4dace6b2 xmlns="f6ca01e7-bd19-41f1-999c-e032ef5104c3">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </m312bc62cb0243b6a873cbbf4dace6b2>
+    <b084a4cb34a444d7969136255594d2f3 xmlns="f6ca01e7-bd19-41f1-999c-e032ef5104c3">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </b084a4cb34a444d7969136255594d2f3>
+    <CreateurAlfresco xmlns="f6ca01e7-bd19-41f1-999c-e032ef5104c3" xsi:nil="true"/>
+    <g30fb2d8061a4d40b63138f91c1a832e xmlns="f6ca01e7-bd19-41f1-999c-e032ef5104c3">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </g30fb2d8061a4d40b63138f91c1a832e>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="1720d4e8-2b1e-4bd1-aad5-1b4debf9b56d">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <m9a76db3058146ae844db6599c9d7036 xmlns="f6ca01e7-bd19-41f1-999c-e032ef5104c3">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </m9a76db3058146ae844db6599c9d7036>
+    <Ticket_x0020_Changement xmlns="f6ca01e7-bd19-41f1-999c-e032ef5104c3" xsi:nil="true"/>
+    <TaxCatchAll xmlns="f6ca01e7-bd19-41f1-999c-e032ef5104c3" xsi:nil="true"/>
+    <l0a6b4600f484920bbceae0813174244 xmlns="f6ca01e7-bd19-41f1-999c-e032ef5104c3">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </l0a6b4600f484920bbceae0813174244>
+  </documentManagement>
+</p:properties>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -14872,69 +14915,56 @@
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <ModificateurAlfresco xmlns="f6ca01e7-bd19-41f1-999c-e032ef5104c3" xsi:nil="true"/>
-    <_ip_UnifiedCompliancePolicyUIAction xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-    <f8b6baa267c0456bbf6a8d18c49a130b xmlns="f6ca01e7-bd19-41f1-999c-e032ef5104c3">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </f8b6baa267c0456bbf6a8d18c49a130b>
-    <eef0f6fc4ed046399a9d01fd3a7d6a6a xmlns="f6ca01e7-bd19-41f1-999c-e032ef5104c3">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </eef0f6fc4ed046399a9d01fd3a7d6a6a>
-    <Référence_x0020_Bon_x0020_de_x0020_Commande xmlns="f6ca01e7-bd19-41f1-999c-e032ef5104c3" xsi:nil="true"/>
-    <Référence_x0020_Documentaire xmlns="f6ca01e7-bd19-41f1-999c-e032ef5104c3" xsi:nil="true"/>
-    <Chantier xmlns="f6ca01e7-bd19-41f1-999c-e032ef5104c3" xsi:nil="true"/>
-    <p671c8df16a44846939d278d4958f62c xmlns="f6ca01e7-bd19-41f1-999c-e032ef5104c3">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </p671c8df16a44846939d278d4958f62c>
-    <Durée_x0020_d_x0027_Utilité_x0020_Administrative_x0020__x0028_DUA_x0029_ xmlns="f6ca01e7-bd19-41f1-999c-e032ef5104c3" xsi:nil="true"/>
-    <Environnement xmlns="f6ca01e7-bd19-41f1-999c-e032ef5104c3" xsi:nil="true"/>
-    <b2804ef99be44b9e8166e80a6c2eb9f1 xmlns="f6ca01e7-bd19-41f1-999c-e032ef5104c3">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </b2804ef99be44b9e8166e80a6c2eb9f1>
-    <_ExtendedDescription xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-    <mc4aa6e782e045f6bb87dab01c971b56 xmlns="f6ca01e7-bd19-41f1-999c-e032ef5104c3">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </mc4aa6e782e045f6bb87dab01c971b56>
-    <_ip_UnifiedCompliancePolicyProperties xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-    <m312bc62cb0243b6a873cbbf4dace6b2 xmlns="f6ca01e7-bd19-41f1-999c-e032ef5104c3">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </m312bc62cb0243b6a873cbbf4dace6b2>
-    <b084a4cb34a444d7969136255594d2f3 xmlns="f6ca01e7-bd19-41f1-999c-e032ef5104c3">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </b084a4cb34a444d7969136255594d2f3>
-    <CreateurAlfresco xmlns="f6ca01e7-bd19-41f1-999c-e032ef5104c3" xsi:nil="true"/>
-    <g30fb2d8061a4d40b63138f91c1a832e xmlns="f6ca01e7-bd19-41f1-999c-e032ef5104c3">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </g30fb2d8061a4d40b63138f91c1a832e>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="1720d4e8-2b1e-4bd1-aad5-1b4debf9b56d">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <m9a76db3058146ae844db6599c9d7036 xmlns="f6ca01e7-bd19-41f1-999c-e032ef5104c3">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </m9a76db3058146ae844db6599c9d7036>
-    <Ticket_x0020_Changement xmlns="f6ca01e7-bd19-41f1-999c-e032ef5104c3" xsi:nil="true"/>
-    <TaxCatchAll xmlns="f6ca01e7-bd19-41f1-999c-e032ef5104c3" xsi:nil="true"/>
-    <l0a6b4600f484920bbceae0813174244 xmlns="f6ca01e7-bd19-41f1-999c-e032ef5104c3">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </l0a6b4600f484920bbceae0813174244>
-  </documentManagement>
-</p:properties>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{475D8938-9E00-42C6-8F04-4B46D606BBA0}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="f6ca01e7-bd19-41f1-999c-e032ef5104c3"/>
+    <ds:schemaRef ds:uri="1720d4e8-2b1e-4bd1-aad5-1b4debf9b56d"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6124D094-6924-4A79-8226-239CA625D903}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
+    <ds:schemaRef ds:uri="f6ca01e7-bd19-41f1-999c-e032ef5104c3"/>
+    <ds:schemaRef ds:uri="1720d4e8-2b1e-4bd1-aad5-1b4debf9b56d"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C5967638-FCD9-44FD-B4E1-300D2A834C2B}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6124D094-6924-4A79-8226-239CA625D903}"/>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{475D8938-9E00-42C6-8F04-4B46D606BBA0}"/>
 </file>
</xml_diff>